<commit_message>
Developed and Changed the testcases
</commit_message>
<xml_diff>
--- a/coxaxle/src/test/resources/datasheets/AT_01_Login.xlsx
+++ b/coxaxle/src/test/resources/datasheets/AT_01_Login.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -23,10 +23,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>sabitha.adama@gmail.com</t>
+    <t>thejaswi.y@vensaiinc.com</t>
   </si>
   <si>
-    <t>qa@123</t>
+    <t>Abc@123</t>
   </si>
 </sst>
 </file>
@@ -900,13 +900,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -928,8 +928,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>